<commit_message>
atualizaçao tempos - ES II
</commit_message>
<xml_diff>
--- a/IPGtrails4health/doc/EngSoft_II/Tabela_Tempos/Tabela_Tempos.xlsx
+++ b/IPGtrails4health/doc/EngSoft_II/Tabela_Tempos/Tabela_Tempos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBP de Rui Windows\Desktop\PI_ESII_Git\IPGtrails4health\IPGtrails4health\doc\EngSoft_II\Tabela_Tempos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo\Documents\GitHub\IPGtrails4health\IPGtrails4health\doc\EngSoft_II\Tabela_Tempos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -186,22 +186,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Cor2" xfId="1" builtinId="34"/>
@@ -534,11 +534,11 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -555,12 +555,14 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>3.5</v>
       </c>
     </row>
@@ -568,9 +570,11 @@
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>3</v>
       </c>
     </row>
@@ -578,9 +582,11 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>0.5</v>
+      </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>2</v>
       </c>
     </row>
@@ -588,9 +594,11 @@
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3">
+        <v>0.5</v>
+      </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>0.5</v>
       </c>
     </row>
@@ -598,15 +606,15 @@
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <f t="shared" ref="C8:D8" si="0">SUM(C4:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="10">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <f>SUM(E4:E7)</f>
         <v>9</v>
       </c>

</xml_diff>